<commit_message>
fixes for spreadsheet validation
</commit_message>
<xml_diff>
--- a/example/test2.xlsx
+++ b/example/test2.xlsx
@@ -998,7 +998,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>"40109c16-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020ef02c-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -1053,7 +1053,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>"4010a0c6-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020ef61c-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -1116,7 +1116,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>"4010a4a4-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020efa0e-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -1171,7 +1171,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>"4010a7f6-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020efd10-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -1230,7 +1230,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>"4010aae4-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020efffe-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>"4010adf0-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f02ec-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -1356,7 +1356,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>"4010b1ce-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f06e8-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1419,7 +1419,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>"4010b53e-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f0a94-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -1482,7 +1482,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>"4010ba0c-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f102a-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1549,7 +1549,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>"4010be12-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f1458-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1604,7 +1604,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>"4010c1c8-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f182c-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>"4010c56a-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f1bec-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1722,7 +1722,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>"4010c9a2-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f204c-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1781,7 +1781,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>"4010ce0c-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f24a2-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1840,7 +1840,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>"4010d186-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f283a-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1895,7 +1895,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>"4010d4f6-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f2bd2-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1954,7 +1954,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>"4010d87a-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f2f6a-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1993,7 +1993,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>"SAXSNEXAFS"</t>
+          <t>"SAXS"</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -2013,7 +2013,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>"4010dbf4-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f32f8-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -2076,7 +2076,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>"4010df64-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f36cc-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -2139,7 +2139,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>"4010e2ca-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f3a5a-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -2182,7 +2182,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>"SAXSNEXAFS"</t>
+          <t>"SAXS"</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -2202,7 +2202,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>"4010e676-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f3e2e-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -2261,7 +2261,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>"4010ea68-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f4248-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -2320,7 +2320,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>"4010ee00-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f4626-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -2359,7 +2359,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>"SAXSNEXAFS"</t>
+          <t>"SAXS"</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2379,7 +2379,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>"4010f18e-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f49e6-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -2438,7 +2438,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>"4010f562-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f4d92-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -2497,7 +2497,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>"4010f940-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f5170-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -2536,7 +2536,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>"SAXSNEXAFS"</t>
+          <t>"SAXS"</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2556,7 +2556,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>"4010fcba-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f5512-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -2615,7 +2615,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>"4011008e-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f5904-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -2674,7 +2674,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>"40111312-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f5cc4-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -2709,7 +2709,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>"SAXSNEXAFS"</t>
+          <t>"WAXS_liquid"</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2729,7 +2729,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>"401116d2-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f6048-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -2784,7 +2784,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>"40111a4c-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f63cc-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -2839,7 +2839,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>"40109efa-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020ef43c-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -2894,7 +2894,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>"4010a2ba-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020ef81a-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -2949,7 +2949,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>"4010a666-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020efb94-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -3012,7 +3012,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>"4010a972-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020efe8c-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -3075,7 +3075,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>"4010ac6a-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f017a-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -3130,7 +3130,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>"4010afe4-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f04f4-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -3193,7 +3193,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>"4010b386-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f08be-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -3256,7 +3256,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>"4010b796-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f0d3c-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -3315,7 +3315,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>"4010bc50-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f1282-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -3378,7 +3378,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>"4010c006-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f1660-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -3432,12 +3432,12 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>"asd"</t>
+          <t>"Carbon"</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>"4010c380-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f19f8-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -3496,7 +3496,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>"4010c790-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f1e1c-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -3555,7 +3555,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>"4010cbaa-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f227c-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -3614,7 +3614,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>"4010cfce-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f266e-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -3669,7 +3669,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>"4010d334-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f2a06-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -3724,7 +3724,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>"4010d6b8-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f2d9e-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -3783,7 +3783,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>"4010da3c-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f312c-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -3826,7 +3826,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>"SAXSNEXAFS"</t>
+          <t>"SAXS"</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -3846,7 +3846,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>"4010ddac-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f3500-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -3909,7 +3909,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>"4010e11c-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f3898-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -3972,7 +3972,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>"4010e482-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f3c26-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -4019,7 +4019,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>"SAXSNEXAFS"</t>
+          <t>"SAXS"</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -4039,7 +4039,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>"4010e87e-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f4054-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -4102,7 +4102,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>"4010ec2a-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f4428-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -4157,7 +4157,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>"4010efe0-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f481a-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -4196,7 +4196,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>"SAXSNEXAFS"</t>
+          <t>"SAXS"</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -4216,7 +4216,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>"4010f346-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f4ba8-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
@@ -4275,7 +4275,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>"4010f74c-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f4f86-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
@@ -4334,7 +4334,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>"4010faf8-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f5346-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
@@ -4369,7 +4369,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>"SAXSNEXAFS"</t>
+          <t>"SAXS_liquid"</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -4389,7 +4389,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>"4010fe72-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f56de-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
@@ -4428,7 +4428,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>"WAXS"</t>
+          <t>"WAXS_liquid"</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -4448,7 +4448,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>"40110246-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f5ad0-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
@@ -4503,7 +4503,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>"4011151a-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f5e90-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
@@ -4538,7 +4538,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>"SAXSNEXAFS"</t>
+          <t>"WAXS_liquid"</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -4558,7 +4558,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>"40111894-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f620a-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
@@ -4593,7 +4593,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>"WAXSNEXAFS"</t>
+          <t>"WAXS_liquid"</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -4613,7 +4613,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>"40111c40-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f658e-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
@@ -4668,7 +4668,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>"40111e0c-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f675a-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
@@ -4723,7 +4723,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>"40111fc4-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f6926-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
@@ -4778,7 +4778,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>"401121c2-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f6b42-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
@@ -4837,7 +4837,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>"401123b6-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f6d36-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
@@ -4896,7 +4896,7 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>"401125aa-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f6f2a-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
@@ -4955,7 +4955,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>"40112794-8f79-11ed-b373-3cecef3aae95"</t>
+          <t>"020f7128-8f7c-11ed-b373-3cecef3aae95"</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">

</xml_diff>